<commit_message>
Changing Extract DataTable from InitAllApplications to GetTransactionData
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V987917\Documents\UiPath\SubstituteItems_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\700024\Documents\UiPath\Projects\UiPath\SubstituteItems_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CF4EAA-47B9-4082-9260-B3A3305C9B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078F9A99-DCB9-421D-842D-123F3F883399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="5265" windowWidth="18315" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -169,6 +169,36 @@
   </si>
   <si>
     <t>The email will receive a notification once the dispatcher or performer ends its process or anything else the process needs.</t>
+  </si>
+  <si>
+    <t>Transaction File (Input File)</t>
+  </si>
+  <si>
+    <t>Sheet_SubstituteItemsName</t>
+  </si>
+  <si>
+    <t>Substitute Items</t>
+  </si>
+  <si>
+    <t>Substitute Items Sheet name</t>
+  </si>
+  <si>
+    <t>File_SubstituteItemsName</t>
+  </si>
+  <si>
+    <t>Input - Substitute Items.xlsx</t>
+  </si>
+  <si>
+    <t>Substitute Items file name (Input file)</t>
+  </si>
+  <si>
+    <t>Sheet_BuyersName</t>
+  </si>
+  <si>
+    <t>Buyers List</t>
+  </si>
+  <si>
+    <t>Buyers list sheet name</t>
   </si>
 </sst>
 </file>
@@ -200,12 +230,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -220,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -230,6 +266,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -628,10 +665,46 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2793,7 +2866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>